<commit_message>
database search with infinite scroll. (excel unfinished)
</commit_message>
<xml_diff>
--- a/database/dwp.xlsx
+++ b/database/dwp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="22">
   <si>
     <t>시간</t>
   </si>
@@ -40,7 +40,7 @@
     <t>운전모드</t>
   </si>
   <si>
-    <t>2015-09-09 11:10</t>
+    <t>2015-11-18 11:40</t>
   </si>
   <si>
     <t>OFF</t>
@@ -49,16 +49,37 @@
     <t>자동</t>
   </si>
   <si>
-    <t>2015-09-09 11:00</t>
-  </si>
-  <si>
-    <t>2015-09-09 10:50</t>
-  </si>
-  <si>
-    <t>2015-09-09 10:40</t>
-  </si>
-  <si>
-    <t>2015-09-09 10:20</t>
+    <t>2015-11-18 11:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:50</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:40</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 09:40</t>
   </si>
 </sst>
 </file>
@@ -407,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,7 +510,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -498,7 +519,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>10</v>
@@ -507,7 +528,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>10</v>
@@ -516,7 +537,7 @@
         <v>9</v>
       </c>
       <c r="L3" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>10</v>
@@ -530,7 +551,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -539,7 +560,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>10</v>
@@ -548,7 +569,7 @@
         <v>9</v>
       </c>
       <c r="I4" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>10</v>
@@ -557,7 +578,7 @@
         <v>9</v>
       </c>
       <c r="L4" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>10</v>
@@ -571,7 +592,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -580,7 +601,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>10</v>
@@ -589,7 +610,7 @@
         <v>9</v>
       </c>
       <c r="I5" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>10</v>
@@ -598,7 +619,7 @@
         <v>9</v>
       </c>
       <c r="L5" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>10</v>
@@ -612,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -621,7 +642,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>10</v>
@@ -630,7 +651,7 @@
         <v>9</v>
       </c>
       <c r="I6" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>10</v>
@@ -639,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="L6" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>10</v>
@@ -653,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -662,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>10</v>
@@ -671,7 +692,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>10</v>
@@ -680,9 +701,296 @@
         <v>9</v>
       </c>
       <c r="L7" s="3">
-        <v>20.79</v>
+        <v>18.44</v>
       </c>
       <c r="M7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="3">
+        <v>18.44</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>